<commit_message>
First pass of demonstrating all of the functionality.
</commit_message>
<xml_diff>
--- a/public/ExampleWorkbook.xlsx
+++ b/public/ExampleWorkbook.xlsx
@@ -5,16 +5,23 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demsu\Projects\vue-excel-example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demsu\Projects\vue-excel-example\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{619D2844-5634-4386-B24E-ABEB12DA5CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FD1281-C62A-45DE-8290-A744C4AA472D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{07616CB8-C6A2-4924-8D80-12B8920C2F69}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{07616CB8-C6A2-4924-8D80-12B8920C2F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table1" sheetId="2" r:id="rId2"/>
+    <sheet name="Route by Name" sheetId="3" r:id="rId3"/>
+    <sheet name="Route by namedRef" sheetId="4" r:id="rId4"/>
+    <sheet name="Route by Function" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="route" localSheetId="3">'Route by namedRef'!$A$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,12 +42,88 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>RouteComponent</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>work!</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>work too!</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>dimensional</t>
+  </si>
+  <si>
+    <t>ranges</t>
+  </si>
+  <si>
+    <t>also</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>yay!</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Dot Warner</t>
+  </si>
+  <si>
+    <t>Yakko Warner</t>
+  </si>
+  <si>
+    <t>dot@warnerbrosandsister.io</t>
+  </si>
+  <si>
+    <t>yakko@warnerbrosandsister.io</t>
+  </si>
+  <si>
+    <t>Wakko Warner</t>
+  </si>
+  <si>
+    <t>wakko@warnerbrosandsister.io</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +146,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -83,6 +169,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB88F41D-F043-48C4-869B-0D8D4F8B816E}" name="Table1" displayName="Table1" ref="A1:C1048576" totalsRowShown="0">
+  <autoFilter ref="A1:C1048576" xr:uid="{EB88F41D-F043-48C4-869B-0D8D4F8B816E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9ED2F1E2-7779-4045-9742-9876F5397D3F}" name="id"/>
+    <tableColumn id="2" xr3:uid="{11D500D0-9407-4ECF-9366-104927CD6519}" name="name"/>
+    <tableColumn id="3" xr3:uid="{060008E2-4E56-4011-9634-94BB2AD8844A}" name="email"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,9 +500,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2027853A-96B4-488E-B0CE-92957BAC2D53}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DB4753-0FED-4158-844E-8636E708E0B3}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="4.265625" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{51E489EA-BA59-47DE-AD15-C1F2817BB683}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{4C67BA9A-3E18-49A4-8FF8-E30C04BD63EB}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{481C4E9F-A993-464B-86A9-D8EC21804813}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D72829-E4D6-437E-A7F8-066B5E5785D9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75ADD548-E982-4A6C-BFE6-292A2F141128}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84607937-238C-4D90-A574-BB703E7E4B4F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>

</xml_diff>

<commit_message>
Additional changes to example workbook
</commit_message>
<xml_diff>
--- a/public/ExampleWorkbook.xlsx
+++ b/public/ExampleWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demsu\Projects\vue-excel-example\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FD1281-C62A-45DE-8290-A744C4AA472D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88E540A-D8CC-49A7-85F1-C3D83ADB831D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{07616CB8-C6A2-4924-8D80-12B8920C2F69}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{07616CB8-C6A2-4924-8D80-12B8920C2F69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>RouteComponent</t>
   </si>
@@ -106,6 +106,42 @@
   </si>
   <si>
     <t>wakko@warnerbrosandsister.io</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>want</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>mount</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>an</t>
+  </si>
+  <si>
+    <t>entire</t>
+  </si>
+  <si>
+    <t>column.</t>
   </si>
 </sst>
 </file>
@@ -500,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2027853A-96B4-488E-B0CE-92957BAC2D53}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -511,7 +547,7 @@
     <col min="3" max="3" width="11.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -521,8 +557,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -535,8 +579,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -549,10 +596,61 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DB4753-0FED-4158-844E-8636E708E0B3}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>